<commit_message>
remove the colum of price weight
</commit_message>
<xml_diff>
--- a/e1.xlsx
+++ b/e1.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -400,15 +400,10 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>قیمت برای ما علیرضا</t>
+          <t>قیمت برای ما</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>قیمت برای ما وزن</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
         <is>
           <t>قیمت برای مشتری</t>
         </is>
@@ -436,9 +431,6 @@
         <v>40000</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
         <v>52000</v>
       </c>
     </row>
@@ -464,9 +456,6 @@
         <v>60000</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
         <v>78000</v>
       </c>
     </row>
@@ -492,9 +481,6 @@
         <v>77000</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
         <v>100100</v>
       </c>
     </row>
@@ -520,9 +506,6 @@
         <v>100000</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
         <v>130000</v>
       </c>
     </row>
@@ -548,9 +531,6 @@
         <v>90000</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
         <v>117000</v>
       </c>
     </row>
@@ -576,9 +556,6 @@
         <v>50000</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
         <v>65000</v>
       </c>
     </row>
@@ -604,9 +581,6 @@
         <v>100000</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
         <v>130000</v>
       </c>
     </row>
@@ -632,9 +606,6 @@
         <v>125000</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
         <v>162500</v>
       </c>
     </row>
@@ -660,9 +631,6 @@
         <v>48000</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
         <v>62400</v>
       </c>
     </row>
@@ -693,7 +661,7 @@
       <c r="F11" t="n">
         <v>180000</v>
       </c>
-      <c r="H11" t="n">
+      <c r="G11" t="n">
         <v>234000</v>
       </c>
     </row>
@@ -724,7 +692,7 @@
       <c r="F12" t="n">
         <v>280000</v>
       </c>
-      <c r="H12" t="n">
+      <c r="G12" t="n">
         <v>364000</v>
       </c>
     </row>
@@ -755,7 +723,7 @@
       <c r="F13" t="n">
         <v>240000</v>
       </c>
-      <c r="H13" t="n">
+      <c r="G13" t="n">
         <v>312000</v>
       </c>
     </row>
@@ -786,7 +754,7 @@
       <c r="F14" t="n">
         <v>130000</v>
       </c>
-      <c r="H14" t="n">
+      <c r="G14" t="n">
         <v>169000</v>
       </c>
     </row>
@@ -817,7 +785,7 @@
       <c r="F15" t="n">
         <v>80000</v>
       </c>
-      <c r="H15" t="n">
+      <c r="G15" t="n">
         <v>104000</v>
       </c>
     </row>
@@ -848,7 +816,7 @@
       <c r="F16" t="n">
         <v>70000</v>
       </c>
-      <c r="H16" t="n">
+      <c r="G16" t="n">
         <v>91000</v>
       </c>
     </row>
@@ -879,7 +847,7 @@
       <c r="F17" t="n">
         <v>230000</v>
       </c>
-      <c r="H17" t="n">
+      <c r="G17" t="n">
         <v>299000</v>
       </c>
     </row>
@@ -910,8 +878,7 @@
       <c r="F18" t="n">
         <v>100000</v>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="n">
+      <c r="G18" t="n">
         <v>130000</v>
       </c>
     </row>

</xml_diff>